<commit_message>
Created unit tests for finding the shortest route
</commit_message>
<xml_diff>
--- a/tests/Test Cases.xlsx
+++ b/tests/Test Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DEF25A-D818-4527-BDE8-EE88AFAF18E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B7C04F-57FC-4A05-9587-0AA47C525B08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Test Case</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Inform 2 airports that are connected thourgh multiple routes with connections</t>
+  </si>
+  <si>
+    <t>Return a 200 HTTP code with the route</t>
+  </si>
+  <si>
+    <t>Return a 200 HTTP code with the shortest route</t>
+  </si>
+  <si>
+    <t>Return a 200 HTTP code with a message</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +476,9 @@
     <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="68.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="67" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -603,9 +614,11 @@
       <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -613,10 +626,10 @@
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -624,7 +637,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -635,7 +648,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>